<commit_message>
Translate test files to English
</commit_message>
<xml_diff>
--- a/src/test/resources/examplefiles/cell-with-error.xlsx
+++ b/src/test/resources/examplefiles/cell-with-error.xlsx
@@ -7,133 +7,138 @@
   </sheets>
   <definedNames/>
   <calcPr/>
+  <extLst>
+    <ext uri="GoogleSheetsCustomDataVersion2">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="cVzeCHq6ywXpPnX7gMr3M3cN8CTYmEtlSrdNHBQTlbI="/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
-    <t>Rad 1, Kol 1</t>
-  </si>
-  <si>
-    <t>Rad 1, Kol 2</t>
-  </si>
-  <si>
-    <t>Rad 1, Kol 3</t>
-  </si>
-  <si>
-    <t>Rad 1, Kol 4</t>
-  </si>
-  <si>
-    <t>Rad 1, Kol 5</t>
-  </si>
-  <si>
-    <t>Rad 1, Kol 6</t>
-  </si>
-  <si>
-    <t>Rad 2, Kol 1</t>
-  </si>
-  <si>
-    <t>Rad 2, Kol 3</t>
-  </si>
-  <si>
-    <t>Rad 2, Kol 4</t>
-  </si>
-  <si>
-    <t>Rad 2, Kol 5</t>
-  </si>
-  <si>
-    <t>Rad 2, Kol 6</t>
-  </si>
-  <si>
-    <t>Rad 3, Kol 1</t>
-  </si>
-  <si>
-    <t>Rad 3, Kol 2</t>
-  </si>
-  <si>
-    <t>Rad 3, Kol 3</t>
-  </si>
-  <si>
-    <t>Rad 3, Kol 4</t>
-  </si>
-  <si>
-    <t>Rad 3, Kol 5</t>
-  </si>
-  <si>
-    <t>Rad 3, Kol 6</t>
-  </si>
-  <si>
-    <t>Rad 4, Kol 1</t>
-  </si>
-  <si>
-    <t>Rad 4, Kol 2</t>
-  </si>
-  <si>
-    <t>Rad 4, Kol 3</t>
-  </si>
-  <si>
-    <t>Rad 4, Kol 4</t>
-  </si>
-  <si>
-    <t>Rad 4, Kol 5</t>
-  </si>
-  <si>
-    <t>Rad 4, Kol 6</t>
-  </si>
-  <si>
-    <t>Rad 5, Kol 1</t>
-  </si>
-  <si>
-    <t>Rad 5, Kol 2</t>
-  </si>
-  <si>
-    <t>Rad 5, Kol 3</t>
-  </si>
-  <si>
-    <t>Rad 5, Kol 4</t>
-  </si>
-  <si>
-    <t>Rad 5, Kol 5</t>
-  </si>
-  <si>
-    <t>Rad 5, Kol 6</t>
-  </si>
-  <si>
-    <t>Rad 6, Kol 1</t>
-  </si>
-  <si>
-    <t>Rad 6, Kol 2</t>
-  </si>
-  <si>
-    <t>Rad 6, Kol 3</t>
-  </si>
-  <si>
-    <t>Rad 6, Kol 4</t>
-  </si>
-  <si>
-    <t>Rad 6, Kol 5</t>
-  </si>
-  <si>
-    <t>Rad 6, Kol 6</t>
-  </si>
-  <si>
-    <t>Rad 7, Kol 1</t>
-  </si>
-  <si>
-    <t>Rad 7, Kol 2</t>
-  </si>
-  <si>
-    <t>Rad 7, Kol 3</t>
-  </si>
-  <si>
-    <t>Rad 7, Kol 4</t>
-  </si>
-  <si>
-    <t>Rad 7, Kol 5</t>
-  </si>
-  <si>
-    <t>Rad 7, Kol 6</t>
+    <t>Row 1, Col 1</t>
+  </si>
+  <si>
+    <t>Row 1, Col 2</t>
+  </si>
+  <si>
+    <t>Row 1, Col 3</t>
+  </si>
+  <si>
+    <t>Row 1, Col 4</t>
+  </si>
+  <si>
+    <t>Row 1, Col 5</t>
+  </si>
+  <si>
+    <t>Row 1, Col 6</t>
+  </si>
+  <si>
+    <t>Row 2, Col 1</t>
+  </si>
+  <si>
+    <t>Row 2, Col 3</t>
+  </si>
+  <si>
+    <t>Row 2, Col 4</t>
+  </si>
+  <si>
+    <t>Row 2, Col 5</t>
+  </si>
+  <si>
+    <t>Row 2, Col 6</t>
+  </si>
+  <si>
+    <t>Row 3, Col 1</t>
+  </si>
+  <si>
+    <t>Row 3, Col 2</t>
+  </si>
+  <si>
+    <t>Row 3, Col 3</t>
+  </si>
+  <si>
+    <t>Row 3, Col 4</t>
+  </si>
+  <si>
+    <t>Row 3, Col 5</t>
+  </si>
+  <si>
+    <t>Row 3, Col 6</t>
+  </si>
+  <si>
+    <t>Row 4, Col 1</t>
+  </si>
+  <si>
+    <t>Row 4, Col 2</t>
+  </si>
+  <si>
+    <t>Row 4, Col 3</t>
+  </si>
+  <si>
+    <t>Row 4, Col 4</t>
+  </si>
+  <si>
+    <t>Row 4, Col 5</t>
+  </si>
+  <si>
+    <t>Row 4, Col 6</t>
+  </si>
+  <si>
+    <t>Row 5, Col 1</t>
+  </si>
+  <si>
+    <t>Row 5, Col 2</t>
+  </si>
+  <si>
+    <t>Row 5, Col 3</t>
+  </si>
+  <si>
+    <t>Row 5, Col 4</t>
+  </si>
+  <si>
+    <t>Row 5, Col 5</t>
+  </si>
+  <si>
+    <t>Row 5, Col 6</t>
+  </si>
+  <si>
+    <t>Row 6, Col 1</t>
+  </si>
+  <si>
+    <t>Row 6, Col 2</t>
+  </si>
+  <si>
+    <t>Row 6, Col 3</t>
+  </si>
+  <si>
+    <t>Row 6, Col 4</t>
+  </si>
+  <si>
+    <t>Row 6, Col 5</t>
+  </si>
+  <si>
+    <t>Row 6, Col 6</t>
+  </si>
+  <si>
+    <t>Row 7, Col 1</t>
+  </si>
+  <si>
+    <t>Row 7, Col 2</t>
+  </si>
+  <si>
+    <t>Row 7, Col 3</t>
+  </si>
+  <si>
+    <t>Row 7, Col 4</t>
+  </si>
+  <si>
+    <t>Row 7, Col 5</t>
+  </si>
+  <si>
+    <t>Row 7, Col 6</t>
   </si>
 </sst>
 </file>
@@ -150,7 +155,6 @@
     <font>
       <color theme="1"/>
       <name val="Arial"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -167,13 +171,14 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -388,13 +393,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="24.88"/>
     <col customWidth="1" min="2" max="2" width="14.0"/>
+    <col customWidth="1" min="3" max="6" width="12.63"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -414,11 +420,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="str">
+      <c r="B2" s="2" t="str">
         <f>iwillcreateanerror</f>
         <v>#NAME?</v>
       </c>
@@ -435,7 +441,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -455,7 +461,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -475,7 +481,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
@@ -495,7 +501,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>29</v>
       </c>
@@ -515,7 +521,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>35</v>
       </c>
@@ -535,6 +541,7 @@
         <v>40</v>
       </c>
     </row>
+    <row r="8" ht="15.75" customHeight="1"/>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>